<commit_message>
Deliv: LAPR3 Assessment update Deliv: ARQCP readme.md added
</commit_message>
<xml_diff>
--- a/deliverables/LAPR3-2023-Self-Assessment_v2.0_2NB_G322_sprint3.xlsx
+++ b/deliverables/LAPR3-2023-Self-Assessment_v2.0_2NB_G322_sprint3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diogoespiritosanto/ESINF/master/deliverables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcaro\PI3\lapr3-2023-2024-group322_main\deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD7351E-9855-BB43-B1D1-E8E233DB78B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684FAA4E-4514-4D47-8AF2-81281E7EAD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="29400" windowHeight="16980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -1744,37 +1744,37 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="19" width="7.83203125" customWidth="1"/>
+    <col min="4" max="19" width="7.875" customWidth="1"/>
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>127</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1785,13 +1785,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:20" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:20" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="E8" s="65" t="s">
@@ -1813,7 +1813,7 @@
       <c r="S8" s="66"/>
       <c r="T8" s="67"/>
     </row>
-    <row r="9" spans="1:20" ht="106" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="105.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="42">
@@ -1880,7 +1880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="62" t="s">
         <v>6</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="63"/>
       <c r="C11" s="8">
         <v>1212044</v>
@@ -1940,15 +1940,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="63"/>
       <c r="C12" s="8">
         <v>1212047</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="35"/>
+      <c r="D12" s="8">
+        <v>4</v>
+      </c>
+      <c r="E12" s="9">
+        <v>3</v>
+      </c>
+      <c r="F12" s="36">
+        <v>4</v>
+      </c>
+      <c r="G12" s="35">
+        <v>5</v>
+      </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -1962,10 +1970,10 @@
       <c r="R12" s="10"/>
       <c r="S12" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="63"/>
       <c r="C13" s="8">
         <v>1221720</v>
@@ -1998,7 +2006,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="63"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -2021,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="63"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
@@ -2044,7 +2052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="63"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -2067,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="63"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
@@ -2090,7 +2098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="63"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -2113,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="63"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -2136,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="63"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -2159,7 +2167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="63"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -2182,7 +2190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="63"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -2205,7 +2213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="63"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -2228,7 +2236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="64"/>
       <c r="C24" s="40"/>
       <c r="D24" s="40"/>
@@ -2251,7 +2259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="45" t="s">
         <v>5</v>
@@ -2262,15 +2270,15 @@
       </c>
       <c r="E25" s="46">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="F25" s="46">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="G25" s="46">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="H25" s="46">
         <f t="shared" si="1"/>
@@ -2318,27 +2326,27 @@
       </c>
       <c r="S25" s="53"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -2346,7 +2354,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2354,7 +2362,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2362,7 +2370,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -2370,7 +2378,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2378,7 +2386,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5</v>
       </c>
@@ -2412,24 +2420,24 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" customWidth="1"/>
     <col min="5" max="10" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>18</v>
       </c>
@@ -2461,7 +2469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="63"/>
       <c r="B4" s="71"/>
       <c r="C4" s="71"/>
@@ -2485,7 +2493,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="63"/>
       <c r="B5" s="71"/>
       <c r="C5" s="71"/>
@@ -2509,14 +2517,16 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>10</v>
       </c>
       <c r="B6" s="29">
         <v>1221720</v>
       </c>
-      <c r="C6" s="29"/>
+      <c r="C6" s="29">
+        <v>4</v>
+      </c>
       <c r="D6" s="60"/>
       <c r="E6" s="31" t="s">
         <v>28</v>
@@ -2537,7 +2547,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>11</v>
       </c>
@@ -2567,7 +2577,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
@@ -2591,7 +2601,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
@@ -2615,7 +2625,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
@@ -2639,7 +2649,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
@@ -2663,7 +2673,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
@@ -2687,7 +2697,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
@@ -2711,7 +2721,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
@@ -2735,7 +2745,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
@@ -2759,7 +2769,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
@@ -2783,7 +2793,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
@@ -2807,7 +2817,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
@@ -2831,7 +2841,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
@@ -2855,7 +2865,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
@@ -2879,7 +2889,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
@@ -2903,7 +2913,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
@@ -2927,7 +2937,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
@@ -2951,7 +2961,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
@@ -2975,7 +2985,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
       <c r="B25" s="54"/>
       <c r="C25" s="54"/>
@@ -3040,28 +3050,28 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.6640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.375" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.83203125" style="1"/>
+    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>37</v>
       </c>
@@ -3080,8 +3090,8 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:26" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:26" ht="48" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>38</v>
       </c>
@@ -3182,7 +3192,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="63" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>40</v>
       </c>
@@ -3193,7 +3203,9 @@
         <v>3</v>
       </c>
       <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="E4" s="25">
+        <v>5</v>
+      </c>
       <c r="F4" s="25">
         <v>4</v>
       </c>
@@ -3210,7 +3222,7 @@
       <c r="Q4" s="25"/>
       <c r="R4" s="27">
         <f t="shared" ref="R4:R7" si="0">AVERAGE(C4:Q4)</f>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="S4" s="7" t="s">
         <v>41</v>
@@ -3233,7 +3245,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="119" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>47</v>
       </c>
@@ -3244,7 +3256,9 @@
         <v>3</v>
       </c>
       <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
+      <c r="E5" s="25">
+        <v>4</v>
+      </c>
       <c r="F5" s="25">
         <v>4</v>
       </c>
@@ -3261,7 +3275,7 @@
       <c r="Q5" s="25"/>
       <c r="R5" s="27">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="S5" s="7" t="s">
         <v>48</v>
@@ -3284,7 +3298,7 @@
       <c r="Y5" s="7"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>54</v>
       </c>
@@ -3295,7 +3309,9 @@
         <v>4</v>
       </c>
       <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
+      <c r="E6" s="25">
+        <v>3</v>
+      </c>
       <c r="F6" s="25">
         <v>4</v>
       </c>
@@ -3312,7 +3328,7 @@
       <c r="Q6" s="25"/>
       <c r="R6" s="27">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="S6" s="7" t="s">
         <v>55</v>
@@ -3335,7 +3351,7 @@
       <c r="Y6" s="7"/>
       <c r="Z6" s="15"/>
     </row>
-    <row r="7" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>60</v>
       </c>
@@ -3346,7 +3362,9 @@
         <v>3</v>
       </c>
       <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
+      <c r="E7" s="25">
+        <v>4</v>
+      </c>
       <c r="F7" s="25">
         <v>4</v>
       </c>
@@ -3363,7 +3381,7 @@
       <c r="Q7" s="25"/>
       <c r="R7" s="27">
         <f t="shared" si="0"/>
-        <v>3.5</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="S7" s="7" t="s">
         <v>61</v>
@@ -3386,7 +3404,7 @@
       <c r="Y7" s="7"/>
       <c r="Z7" s="15"/>
     </row>
-    <row r="8" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>36</v>
       </c>
@@ -3404,7 +3422,7 @@
       </c>
       <c r="E8" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.5999999999999996</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="1"/>
@@ -3464,7 +3482,7 @@
       <c r="Y8" s="7"/>
       <c r="Z8" s="15"/>
     </row>
-    <row r="9" spans="1:26" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>66</v>
       </c>
@@ -3479,7 +3497,7 @@
       </c>
       <c r="E9" s="23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>14.399999999999999</v>
       </c>
       <c r="F9" s="23">
         <f t="shared" si="2"/>
@@ -3539,7 +3557,7 @@
       <c r="Y9" s="23"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
     </row>
   </sheetData>
@@ -3559,25 +3577,25 @@
   <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.6640625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="20.6640625" style="1" customWidth="1"/>
+    <col min="22" max="24" width="20.625" style="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.83203125" style="1"/>
+    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>67</v>
       </c>
@@ -3596,7 +3614,7 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="3" spans="1:26" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="48" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>38</v>
       </c>
@@ -3697,7 +3715,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>68</v>
       </c>
@@ -3708,7 +3726,9 @@
         <v>4</v>
       </c>
       <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="E4" s="25">
+        <v>5</v>
+      </c>
       <c r="F4" s="25">
         <v>4</v>
       </c>
@@ -3725,7 +3745,7 @@
       <c r="Q4" s="25"/>
       <c r="R4" s="55">
         <f t="shared" ref="R4:R7" si="0">AVERAGE(C4:Q4)</f>
-        <v>4</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="S4" s="59" t="s">
         <v>69</v>
@@ -3748,7 +3768,7 @@
       <c r="Y4" s="56"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>75</v>
       </c>
@@ -3759,7 +3779,9 @@
         <v>4</v>
       </c>
       <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
+      <c r="E5" s="25">
+        <v>4</v>
+      </c>
       <c r="F5" s="25">
         <v>4</v>
       </c>
@@ -3799,7 +3821,7 @@
       <c r="Y5" s="56"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>82</v>
       </c>
@@ -3810,7 +3832,9 @@
         <v>5</v>
       </c>
       <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
+      <c r="E6" s="25">
+        <v>5</v>
+      </c>
       <c r="F6" s="25">
         <v>5</v>
       </c>
@@ -3850,7 +3874,7 @@
       <c r="Y6" s="56"/>
       <c r="Z6" s="15"/>
     </row>
-    <row r="7" spans="1:26" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>89</v>
       </c>
@@ -3861,7 +3885,9 @@
         <v>4</v>
       </c>
       <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
+      <c r="E7" s="25">
+        <v>5</v>
+      </c>
       <c r="F7" s="25">
         <v>5</v>
       </c>
@@ -3878,7 +3904,7 @@
       <c r="Q7" s="25"/>
       <c r="R7" s="55">
         <f t="shared" si="0"/>
-        <v>4.5</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="S7" s="59" t="s">
         <v>83</v>
@@ -3901,7 +3927,7 @@
       <c r="Y7" s="56"/>
       <c r="Z7" s="15"/>
     </row>
-    <row r="8" spans="1:26" ht="68" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="63" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>95</v>
       </c>
@@ -3912,7 +3938,9 @@
         <v>4</v>
       </c>
       <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
+      <c r="E8" s="25">
+        <v>5</v>
+      </c>
       <c r="F8" s="25">
         <v>5</v>
       </c>
@@ -3929,7 +3957,7 @@
       <c r="Q8" s="25"/>
       <c r="R8" s="55">
         <f t="shared" ref="R8:R12" si="1">AVERAGE(C8:Q8)</f>
-        <v>4.5</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="S8" s="59" t="s">
         <v>83</v>
@@ -3952,7 +3980,7 @@
       <c r="Y8" s="56"/>
       <c r="Z8" s="15"/>
     </row>
-    <row r="9" spans="1:26" ht="68" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>101</v>
       </c>
@@ -3963,7 +3991,9 @@
         <v>4</v>
       </c>
       <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
+      <c r="E9" s="25">
+        <v>4</v>
+      </c>
       <c r="F9" s="25">
         <v>4</v>
       </c>
@@ -3999,7 +4029,7 @@
       <c r="Y9" s="56"/>
       <c r="Z9" s="15"/>
     </row>
-    <row r="10" spans="1:26" ht="102" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>106</v>
       </c>
@@ -4010,7 +4040,9 @@
         <v>4</v>
       </c>
       <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
+      <c r="E10" s="25">
+        <v>5</v>
+      </c>
       <c r="F10" s="25">
         <v>4</v>
       </c>
@@ -4027,7 +4059,7 @@
       <c r="Q10" s="25"/>
       <c r="R10" s="55">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="S10" s="59" t="s">
         <v>102</v>
@@ -4050,7 +4082,7 @@
       <c r="Y10" s="56"/>
       <c r="Z10" s="15"/>
     </row>
-    <row r="11" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>112</v>
       </c>
@@ -4061,7 +4093,9 @@
         <v>3</v>
       </c>
       <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
+      <c r="E11" s="25">
+        <v>3</v>
+      </c>
       <c r="F11" s="25">
         <v>3</v>
       </c>
@@ -4101,7 +4135,7 @@
       <c r="Y11" s="56"/>
       <c r="Z11" s="15"/>
     </row>
-    <row r="12" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>118</v>
       </c>
@@ -4112,7 +4146,9 @@
         <v>3</v>
       </c>
       <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
+      <c r="E12" s="25">
+        <v>4</v>
+      </c>
       <c r="F12" s="25">
         <v>4</v>
       </c>
@@ -4129,7 +4165,7 @@
       <c r="Q12" s="25"/>
       <c r="R12" s="55">
         <f t="shared" si="1"/>
-        <v>3.5</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="S12" s="59" t="s">
         <v>102</v>
@@ -4152,7 +4188,7 @@
       <c r="Y12" s="56"/>
       <c r="Z12" s="15"/>
     </row>
-    <row r="13" spans="1:26" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>119</v>
       </c>
@@ -4163,7 +4199,9 @@
         <v>3</v>
       </c>
       <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
+      <c r="E13" s="25">
+        <v>4</v>
+      </c>
       <c r="F13" s="25">
         <v>4</v>
       </c>
@@ -4180,7 +4218,7 @@
       <c r="Q13" s="25"/>
       <c r="R13" s="55">
         <f t="shared" ref="R13:R14" si="3">AVERAGE(C13:Q13)</f>
-        <v>3.5</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="S13" s="59" t="s">
         <v>120</v>
@@ -4203,7 +4241,7 @@
       <c r="Y13" s="56"/>
       <c r="Z13" s="15"/>
     </row>
-    <row r="14" spans="1:26" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>126</v>
       </c>
@@ -4214,7 +4252,9 @@
         <v>3</v>
       </c>
       <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
+      <c r="E14" s="25">
+        <v>4</v>
+      </c>
       <c r="F14" s="25">
         <v>4</v>
       </c>
@@ -4231,7 +4271,7 @@
       <c r="Q14" s="25"/>
       <c r="R14" s="55">
         <f t="shared" si="3"/>
-        <v>3.5</v>
+        <v>3.6666666666666665</v>
       </c>
       <c r="S14" s="59" t="s">
         <v>102</v>
@@ -4254,7 +4294,7 @@
       <c r="Y14" s="56"/>
       <c r="Z14" s="15"/>
     </row>
-    <row r="15" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>36</v>
       </c>
@@ -4272,7 +4312,7 @@
       </c>
       <c r="E15" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4.3</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="4"/>
@@ -4332,7 +4372,7 @@
       <c r="Y15" s="7"/>
       <c r="Z15" s="15"/>
     </row>
-    <row r="16" spans="1:26" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>66</v>
       </c>
@@ -4347,7 +4387,7 @@
       </c>
       <c r="E16" s="23">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>17.2</v>
       </c>
       <c r="F16" s="23">
         <f t="shared" si="5"/>
@@ -4407,7 +4447,7 @@
       <c r="Y16" s="23"/>
       <c r="Z16" s="16"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
     </row>
   </sheetData>
@@ -4431,6 +4471,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
     <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
@@ -4614,12 +4660,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
   <ds:schemaRefs>
@@ -4629,6 +4669,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B77F7C-EE47-4FBD-B078-6536C1487A1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4645,20 +4701,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
LAPR - Self-assessment correction
</commit_message>
<xml_diff>
--- a/deliverables/LAPR3-2023-Self-Assessment_v2.0_2NB_G322_sprint3.xlsx
+++ b/deliverables/LAPR3-2023-Self-Assessment_v2.0_2NB_G322_sprint3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulo\Desktop\lapr3-2023-2024-group322_main\deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45320177-60F3-4CD7-A72A-7AC9AFA1889B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3DA992-7437-4E83-A093-EC3DCA5B2276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1097" yWindow="1097" windowWidth="24686" windowHeight="13054" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3590,10 +3590,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:Z17"/>
+  <dimension ref="A1:Z49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -4487,6 +4487,11 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="5"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D49" s="1">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -4509,12 +4514,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
     <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
@@ -4698,6 +4697,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
   <ds:schemaRefs>
@@ -4707,22 +4712,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B77F7C-EE47-4FBD-B078-6536C1487A1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4739,4 +4728,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>